<commit_message>
prepare for modify model
</commit_message>
<xml_diff>
--- a/Assets/DataProcessing/Speed_Err.xlsx
+++ b/Assets/DataProcessing/Speed_Err.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\Keyboard\Assets\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E610CA8-F8A0-4E0A-BA61-44D61E9DC6D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD737550-F954-4937-9A05-652D6477C7F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13212" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -75,21 +75,21 @@
   </si>
   <si>
     <t>zzc</t>
-  </si>
-  <si>
-    <t>SKPad</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>FanPad</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>crossover</t>
+    <t>NSPad</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nocrossover</t>
+    <t>NSPad+Crossover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FanPad+Crossover</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -440,7 +440,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+      <selection activeCell="D1" sqref="D1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -950,7 +952,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D2" sqref="D2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1208,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D2" sqref="D2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1459,83 +1461,522 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
       </c>
       <c r="B2">
         <v>8.0696250000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="D2">
+        <v>7.0921985815602844E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>5.5237045299999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.25766871165644167</v>
+      </c>
+      <c r="D3">
+        <v>6.1349693251533744E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>9.5543250000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0.1595092024539877</v>
+      </c>
+      <c r="D4">
+        <v>2.4539877300613501E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>9.5789139999999993</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1.515151515151515E-2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>9.3031225200000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0.11971830985915489</v>
+      </c>
+      <c r="D6">
+        <v>7.0422535211267607E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>10.9330654</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0.17123287671232881</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>8.6586759999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>6.2893081761006289E-2</v>
+      </c>
+      <c r="D8">
+        <v>6.2893081761006293E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7.1625804899999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.1019108280254777</v>
+      </c>
+      <c r="D9">
+        <v>1.2738853503184711E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>11.470965400000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>6.7114093959731542E-3</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9.8345350000000007</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>9.9378881987577633E-2</v>
+      </c>
+      <c r="D11">
+        <v>6.2111801242236021E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>6.5955029999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3.6496350364963501E-2</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
+      </c>
+      <c r="B13">
+        <v>8.5912609999999994</v>
+      </c>
+      <c r="C13">
+        <v>4.3209876543209867E-2</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6.8755564700000003</v>
+      </c>
+      <c r="C14">
+        <v>0.13529411764705879</v>
+      </c>
+      <c r="D14">
+        <v>1.1764705882352939E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>11.762828799999999</v>
+      </c>
+      <c r="C15">
+        <v>4.9295774647887321E-2</v>
+      </c>
+      <c r="D15">
+        <v>2.1126760563380281E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>9.1712140000000009</v>
+      </c>
+      <c r="C16">
+        <v>0.1076923076923077</v>
+      </c>
+      <c r="D16">
+        <v>7.6923076923076927E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>7.86100054</v>
+      </c>
+      <c r="C17">
+        <v>0.27142857142857141</v>
+      </c>
+      <c r="D17">
+        <v>7.1428571428571426E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>12.3066473</v>
+      </c>
+      <c r="C18">
+        <v>0.14482758620689659</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>9.7173339999999993</v>
+      </c>
+      <c r="C19">
+        <v>6.535947712418301E-2</v>
+      </c>
+      <c r="D19">
+        <v>3.2679738562091512E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>6.7439217600000001</v>
+      </c>
+      <c r="C20">
+        <v>0.19108280254777071</v>
+      </c>
+      <c r="D20">
+        <v>1.2738853503184711E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>12.3341236</v>
+      </c>
+      <c r="C21">
+        <v>4.2253521126760563E-2</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>9.8494410000000006</v>
+      </c>
+      <c r="C22">
+        <v>0.1714285714285714</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>8.6107650000000007</v>
+      </c>
+      <c r="C23">
+        <v>4.0268456375838917E-2</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>8.5382680000000004</v>
+      </c>
+      <c r="C24">
+        <v>8.0882352941176475E-2</v>
+      </c>
+      <c r="D24">
+        <v>2.9411764705882349E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>5.7163252800000004</v>
+      </c>
+      <c r="C25">
+        <v>0.39333333333333331</v>
+      </c>
+      <c r="D25">
+        <v>1.3333333333333331E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>9.0767330000000008</v>
+      </c>
+      <c r="C26">
+        <v>7.7519379844961239E-2</v>
+      </c>
+      <c r="D26">
+        <v>7.7519379844961239E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>7.05044746</v>
+      </c>
+      <c r="C27">
+        <v>0.1586206896551724</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>10.148740800000001</v>
+      </c>
+      <c r="C28">
+        <v>0.28484848484848491</v>
+      </c>
+      <c r="D28">
+        <v>0.1393939393939394</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>13.8219709</v>
+      </c>
+      <c r="C29">
+        <v>4.9645390070921988E-2</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>8.3716489999999997</v>
+      </c>
+      <c r="C30">
+        <v>0.14285714285714279</v>
+      </c>
+      <c r="D30">
+        <v>1.298701298701299E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>6.7104725800000002</v>
+      </c>
+      <c r="C31">
+        <v>0.19886363636363641</v>
+      </c>
+      <c r="D31">
+        <v>1.7045454545454541E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>13.1038227</v>
+      </c>
+      <c r="C32">
+        <v>3.870967741935484E-2</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>12.301046400000001</v>
+      </c>
+      <c r="C33">
+        <v>0.08</v>
+      </c>
+      <c r="D33">
+        <v>1.3333333333333331E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>8.4806869999999996</v>
+      </c>
+      <c r="C34">
+        <v>0.16058394160583939</v>
+      </c>
+      <c r="D34">
+        <v>5.8394160583941597E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>8.1561760000000003</v>
+      </c>
+      <c r="C35">
+        <v>7.9710144927536225E-2</v>
+      </c>
+      <c r="D35">
+        <v>2.1739130434782612E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>6.6420693399999999</v>
+      </c>
+      <c r="C36">
+        <v>0.34567901234567899</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>9.4187329999999996</v>
+      </c>
+      <c r="C37">
+        <v>7.8014184397163122E-2</v>
+      </c>
+      <c r="D37">
+        <v>1.4184397163120571E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>10.4880228</v>
+      </c>
+      <c r="C38">
+        <v>3.0769230769230771E-2</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>7.2268840000000001</v>
+      </c>
+      <c r="C39">
+        <v>0.24305555555555561</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>13.6694613</v>
+      </c>
+      <c r="C40">
+        <v>6.993006993006993E-3</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>9.7924989999999994</v>
+      </c>
+      <c r="C41">
+        <v>4.4117647058823532E-2</v>
+      </c>
+      <c r="D41">
+        <v>7.3529411764705881E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>6.8696229999999998</v>
+      </c>
+      <c r="C42">
+        <v>0.16265060240963861</v>
+      </c>
+      <c r="D42">
+        <v>6.024096385542169E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>14.006744400000001</v>
+      </c>
+      <c r="C43">
+        <v>0.15822784810126581</v>
+      </c>
+      <c r="D43">
+        <v>2.5316455696202531E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>8.9695219999999996</v>
+      </c>
+      <c r="C44">
+        <v>0.1437908496732026</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>9.73522</v>
+      </c>
+      <c r="C45">
+        <v>0.1176470588235294</v>
+      </c>
+      <c r="D45">
+        <v>5.8823529411764714E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ppt and experiment data
</commit_message>
<xml_diff>
--- a/Assets/DataProcessing/Speed_Err.xlsx
+++ b/Assets/DataProcessing/Speed_Err.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\Keyboard\Assets\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E610CA8-F8A0-4E0A-BA61-44D61E9DC6D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC368D93-7B96-4FD7-975F-CDF9536A2D50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13212" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -90,6 +90,130 @@
   </si>
   <si>
     <t>nocrossover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方差分析：可重复双因素分析</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>SKPad</t>
+  </si>
+  <si>
+    <t>FanPad</t>
+  </si>
+  <si>
+    <t>总计</t>
+  </si>
+  <si>
+    <t>nocrossover</t>
+  </si>
+  <si>
+    <t>观测数</t>
+  </si>
+  <si>
+    <t>求和</t>
+  </si>
+  <si>
+    <t>平均</t>
+  </si>
+  <si>
+    <t>方差</t>
+  </si>
+  <si>
+    <t>crossover</t>
+  </si>
+  <si>
+    <t>方差分析</t>
+  </si>
+  <si>
+    <t>差异源</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>F crit</t>
+  </si>
+  <si>
+    <t>样本</t>
+  </si>
+  <si>
+    <t>列</t>
+  </si>
+  <si>
+    <t>交互</t>
+  </si>
+  <si>
+    <t>内部</t>
+  </si>
+  <si>
+    <t>WPM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t-检验: 成对双样本均值分析</t>
+  </si>
+  <si>
+    <t>观测值</t>
+  </si>
+  <si>
+    <t>泊松相关系数</t>
+  </si>
+  <si>
+    <t>假设平均差</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) 单尾</t>
+  </si>
+  <si>
+    <t>t 单尾临界</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) 双尾</t>
+  </si>
+  <si>
+    <t>t 双尾临界</t>
+  </si>
+  <si>
+    <t>NSPad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FanPad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nocrossover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crossover</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -121,7 +245,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -129,12 +253,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -440,7 +604,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+      <selection activeCell="F2" sqref="F2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -695,7 +859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -950,7 +1116,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F2" sqref="F2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1372,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F2" sqref="F2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1459,86 +1625,1858 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:W86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="Q1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>8.0696250000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="C3">
+        <v>8.5382680000000004</v>
+      </c>
+      <c r="E3">
+        <v>8.0696250000000003</v>
+      </c>
+      <c r="F3">
+        <v>8.5912609999999994</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="K3">
+        <v>8.0882352941176475E-2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3">
+        <v>7.0921985815602844E-3</v>
+      </c>
+      <c r="S3">
+        <v>2.9411764705882349E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>5.5237045299999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="C4">
+        <v>5.7163252800000004</v>
+      </c>
+      <c r="E4">
+        <v>5.5237045299999998</v>
+      </c>
+      <c r="F4">
+        <v>6.8755564700000003</v>
+      </c>
+      <c r="J4">
+        <v>0.25766871165644167</v>
+      </c>
+      <c r="K4">
+        <v>0.39333333333333331</v>
+      </c>
+      <c r="R4">
+        <v>6.1349693251533744E-3</v>
+      </c>
+      <c r="S4">
+        <v>1.3333333333333331E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>9.5543250000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="C5">
+        <v>9.0767330000000008</v>
+      </c>
+      <c r="E5">
+        <v>9.5543250000000004</v>
+      </c>
+      <c r="F5">
+        <v>11.762828799999999</v>
+      </c>
+      <c r="J5">
+        <v>0.1595092024539877</v>
+      </c>
+      <c r="K5">
+        <v>7.7519379844961239E-2</v>
+      </c>
+      <c r="R5">
+        <v>2.4539877300613501E-2</v>
+      </c>
+      <c r="S5">
+        <v>7.7519379844961239E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>9.5789139999999993</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="C6">
+        <v>7.05044746</v>
+      </c>
+      <c r="E6">
+        <v>9.5789139999999993</v>
+      </c>
+      <c r="F6">
+        <v>9.1712140000000009</v>
+      </c>
+      <c r="J6">
+        <v>1.515151515151515E-2</v>
+      </c>
+      <c r="K6">
+        <v>0.1586206896551724</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>9.3031225200000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="C7">
+        <v>10.148740800000001</v>
+      </c>
+      <c r="E7">
+        <v>9.3031225200000005</v>
+      </c>
+      <c r="F7">
+        <v>7.86100054</v>
+      </c>
+      <c r="J7">
+        <v>0.11971830985915489</v>
+      </c>
+      <c r="K7">
+        <v>0.28484848484848491</v>
+      </c>
+      <c r="R7">
+        <v>7.0422535211267607E-3</v>
+      </c>
+      <c r="S7">
+        <v>0.1393939393939394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>10.9330654</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="C8">
+        <v>13.8219709</v>
+      </c>
+      <c r="E8">
+        <v>10.9330654</v>
+      </c>
+      <c r="F8">
+        <v>12.3066473</v>
+      </c>
+      <c r="J8">
+        <v>0.17123287671232881</v>
+      </c>
+      <c r="K8">
+        <v>4.9645390070921988E-2</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>8.6586759999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="C9">
+        <v>8.3716489999999997</v>
+      </c>
+      <c r="E9">
+        <v>8.6586759999999998</v>
+      </c>
+      <c r="F9">
+        <v>9.7173339999999993</v>
+      </c>
+      <c r="J9">
+        <v>6.2893081761006289E-2</v>
+      </c>
+      <c r="K9">
+        <v>0.14285714285714279</v>
+      </c>
+      <c r="R9">
+        <v>6.2893081761006293E-3</v>
+      </c>
+      <c r="S9">
+        <v>1.298701298701299E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>7.1625804899999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="C10">
+        <v>6.7104725800000002</v>
+      </c>
+      <c r="E10">
+        <v>7.1625804899999999</v>
+      </c>
+      <c r="F10">
+        <v>6.7439217600000001</v>
+      </c>
+      <c r="J10">
+        <v>0.1019108280254777</v>
+      </c>
+      <c r="K10">
+        <v>0.19886363636363641</v>
+      </c>
+      <c r="R10">
+        <v>1.2738853503184711E-2</v>
+      </c>
+      <c r="S10">
+        <v>1.7045454545454541E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>11.470965400000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="C11">
+        <v>13.1038227</v>
+      </c>
+      <c r="E11">
+        <v>11.470965400000001</v>
+      </c>
+      <c r="F11">
+        <v>12.3341236</v>
+      </c>
+      <c r="J11">
+        <v>6.7114093959731542E-3</v>
+      </c>
+      <c r="K11">
+        <v>3.870967741935484E-2</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>9.8345350000000007</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="C12">
+        <v>12.301046400000001</v>
+      </c>
+      <c r="E12">
+        <v>9.8345350000000007</v>
+      </c>
+      <c r="F12">
+        <v>9.8494410000000006</v>
+      </c>
+      <c r="J12">
+        <v>9.9378881987577633E-2</v>
+      </c>
+      <c r="K12">
+        <v>0.08</v>
+      </c>
+      <c r="R12">
+        <v>6.2111801242236021E-3</v>
+      </c>
+      <c r="S12">
+        <v>1.3333333333333331E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13">
         <v>6.5955029999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13">
+        <v>8.4806869999999996</v>
+      </c>
+      <c r="E13">
+        <v>6.5955029999999999</v>
+      </c>
+      <c r="F13">
+        <v>8.6107650000000007</v>
+      </c>
+      <c r="J13">
+        <v>3.6496350364963501E-2</v>
+      </c>
+      <c r="K13">
+        <v>0.16058394160583939</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>5.8394160583941597E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
+      <c r="B14">
+        <v>8.5912609999999994</v>
+      </c>
+      <c r="C14">
+        <v>8.1561760000000003</v>
+      </c>
+      <c r="E14">
+        <v>8.5382680000000004</v>
+      </c>
+      <c r="F14">
+        <v>8.1561760000000003</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14">
+        <v>4.3209876543209867E-2</v>
+      </c>
+      <c r="K14">
+        <v>7.9710144927536225E-2</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>2.1739130434782612E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>6.8755564700000003</v>
+      </c>
+      <c r="C15">
+        <v>6.6420693399999999</v>
+      </c>
+      <c r="E15">
+        <v>5.7163252800000004</v>
+      </c>
+      <c r="F15">
+        <v>6.6420693399999999</v>
+      </c>
+      <c r="J15">
+        <v>0.13529411764705879</v>
+      </c>
+      <c r="K15">
+        <v>0.34567901234567899</v>
+      </c>
+      <c r="R15">
+        <v>1.1764705882352939E-2</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>11.762828799999999</v>
+      </c>
+      <c r="C16">
+        <v>9.4187329999999996</v>
+      </c>
+      <c r="E16">
+        <v>9.0767330000000008</v>
+      </c>
+      <c r="F16">
+        <v>9.4187329999999996</v>
+      </c>
+      <c r="J16">
+        <v>4.9295774647887321E-2</v>
+      </c>
+      <c r="K16">
+        <v>7.8014184397163122E-2</v>
+      </c>
+      <c r="R16">
+        <v>2.1126760563380281E-2</v>
+      </c>
+      <c r="S16">
+        <v>1.4184397163120571E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>9.1712140000000009</v>
+      </c>
+      <c r="C17">
+        <v>10.4880228</v>
+      </c>
+      <c r="E17">
+        <v>7.05044746</v>
+      </c>
+      <c r="F17">
+        <v>10.4880228</v>
+      </c>
+      <c r="J17">
+        <v>0.1076923076923077</v>
+      </c>
+      <c r="K17">
+        <v>3.0769230769230771E-2</v>
+      </c>
+      <c r="R17">
+        <v>7.6923076923076927E-3</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>7.86100054</v>
+      </c>
+      <c r="C18">
+        <v>7.2268840000000001</v>
+      </c>
+      <c r="E18">
+        <v>10.148740800000001</v>
+      </c>
+      <c r="F18">
+        <v>7.2268840000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.27142857142857141</v>
+      </c>
+      <c r="K18">
+        <v>0.24305555555555561</v>
+      </c>
+      <c r="R18">
+        <v>7.1428571428571426E-3</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>12.3066473</v>
+      </c>
+      <c r="C19">
+        <v>13.6694613</v>
+      </c>
+      <c r="E19">
+        <v>13.8219709</v>
+      </c>
+      <c r="F19">
+        <v>13.6694613</v>
+      </c>
+      <c r="J19">
+        <v>0.14482758620689659</v>
+      </c>
+      <c r="K19">
+        <v>6.993006993006993E-3</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>9.7173339999999993</v>
+      </c>
+      <c r="C20">
+        <v>9.7924989999999994</v>
+      </c>
+      <c r="E20">
+        <v>8.3716489999999997</v>
+      </c>
+      <c r="F20">
+        <v>9.7924989999999994</v>
+      </c>
+      <c r="J20">
+        <v>6.535947712418301E-2</v>
+      </c>
+      <c r="K20">
+        <v>4.4117647058823532E-2</v>
+      </c>
+      <c r="R20">
+        <v>3.2679738562091512E-2</v>
+      </c>
+      <c r="S20">
+        <v>7.3529411764705881E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>6.7439217600000001</v>
+      </c>
+      <c r="C21">
+        <v>6.8696229999999998</v>
+      </c>
+      <c r="E21">
+        <v>6.7104725800000002</v>
+      </c>
+      <c r="F21">
+        <v>6.8696229999999998</v>
+      </c>
+      <c r="J21">
+        <v>0.19108280254777071</v>
+      </c>
+      <c r="K21">
+        <v>0.16265060240963861</v>
+      </c>
+      <c r="R21">
+        <v>1.2738853503184711E-2</v>
+      </c>
+      <c r="S21">
+        <v>6.024096385542169E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>12.3341236</v>
+      </c>
+      <c r="C22">
+        <v>14.006744400000001</v>
+      </c>
+      <c r="E22">
+        <v>13.1038227</v>
+      </c>
+      <c r="F22">
+        <v>14.006744400000001</v>
+      </c>
+      <c r="J22">
+        <v>4.2253521126760563E-2</v>
+      </c>
+      <c r="K22">
+        <v>0.15822784810126581</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>2.5316455696202531E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>9.8494410000000006</v>
+      </c>
+      <c r="C23">
+        <v>8.9695219999999996</v>
+      </c>
+      <c r="E23">
+        <v>12.301046400000001</v>
+      </c>
+      <c r="F23">
+        <v>8.9695219999999996</v>
+      </c>
+      <c r="J23">
+        <v>0.1714285714285714</v>
+      </c>
+      <c r="K23">
+        <v>0.1437908496732026</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>8.6107650000000007</v>
+      </c>
+      <c r="C24">
+        <v>9.73522</v>
+      </c>
+      <c r="E24">
+        <v>8.4806869999999996</v>
+      </c>
+      <c r="F24">
+        <v>9.73522</v>
+      </c>
+      <c r="J24">
+        <v>4.0268456375838917E-2</v>
+      </c>
+      <c r="K24">
+        <v>0.1176470588235294</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>5.8823529411764714E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>22</v>
+      </c>
+      <c r="R29" t="s">
+        <v>23</v>
+      </c>
+      <c r="S29" t="s">
+        <v>24</v>
+      </c>
+      <c r="T29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="I30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="Q30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1">
+        <v>22</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" s="1">
+        <v>11</v>
+      </c>
+      <c r="K31" s="1">
+        <v>11</v>
+      </c>
+      <c r="L31" s="1">
+        <v>22</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R31" s="1">
+        <v>11</v>
+      </c>
+      <c r="S31" s="1">
+        <v>11</v>
+      </c>
+      <c r="T31" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1">
+        <v>96.68501633999999</v>
+      </c>
+      <c r="C32" s="1">
+        <v>103.32016312</v>
+      </c>
+      <c r="D32" s="1">
+        <v>200.00517945999997</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="1">
+        <v>1.0732243588577883</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1.6658640289400239</v>
+      </c>
+      <c r="L32" s="1">
+        <v>2.7390883877978118</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R32" s="1">
+        <v>7.0048640531962858E-2</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0.29165093686739368</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0.36169957739935649</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8.7895469399999993</v>
+      </c>
+      <c r="C33" s="1">
+        <v>9.3927421018181825</v>
+      </c>
+      <c r="D33" s="1">
+        <v>9.09114452090909</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33" s="1">
+        <v>9.7565850805253485E-2</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.15144218444909308</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.12450401762717327</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R33" s="1">
+        <v>6.3680582301784416E-3</v>
+      </c>
+      <c r="S33" s="1">
+        <v>2.6513721533399426E-2</v>
+      </c>
+      <c r="T33" s="1">
+        <v>1.644088988178893E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3.3010412194035781</v>
+      </c>
+      <c r="C34" s="1">
+        <v>7.1321372874275877</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5.0634728231494011</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J34" s="1">
+        <v>5.8414362650722525E-3</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1.1738463066522204E-2</v>
+      </c>
+      <c r="L34" s="1">
+        <v>9.1316009339955963E-3</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R34" s="1">
+        <v>5.3407476451858725E-5</v>
+      </c>
+      <c r="S34" s="1">
+        <v>1.6847706633178489E-3</v>
+      </c>
+      <c r="T34" s="1">
+        <v>9.339973343949605E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="I36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="Q36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="1">
+        <v>11</v>
+      </c>
+      <c r="C37" s="1">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1">
+        <v>22</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J37" s="1">
+        <v>11</v>
+      </c>
+      <c r="K37" s="1">
+        <v>11</v>
+      </c>
+      <c r="L37" s="1">
+        <v>22</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R37" s="1">
+        <v>11</v>
+      </c>
+      <c r="S37" s="1">
+        <v>11</v>
+      </c>
+      <c r="T37" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="1">
+        <v>103.82409346999999</v>
+      </c>
+      <c r="C38" s="1">
+        <v>104.97495484000001</v>
+      </c>
+      <c r="D38" s="1">
+        <v>208.79904831000002</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1.2621410627690561</v>
+      </c>
+      <c r="K38" s="1">
+        <v>1.4106551410546315</v>
+      </c>
+      <c r="L38" s="1">
+        <v>2.6727962038236881</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R38" s="1">
+        <v>9.3145223346174283E-2</v>
+      </c>
+      <c r="S38" s="1">
+        <v>8.0499373797294951E-2</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0.17364459714346922</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="1">
+        <v>9.4385539518181805</v>
+      </c>
+      <c r="C39" s="1">
+        <v>9.5431777127272728</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9.4908658322727284</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.11474009661536874</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0.12824137645951195</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0.12149073653744037</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R39" s="1">
+        <v>8.4677475769249343E-3</v>
+      </c>
+      <c r="S39" s="1">
+        <v>7.3181248906631774E-3</v>
+      </c>
+      <c r="T39" s="1">
+        <v>7.892936233794055E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="1">
+        <v>4.0052367145794507</v>
+      </c>
+      <c r="C40" s="1">
+        <v>6.1139299667911589</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4.8215176445768346</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J40" s="1">
+        <v>5.7608772272931263E-3</v>
+      </c>
+      <c r="K40" s="1">
+        <v>9.9055469605179771E-3</v>
+      </c>
+      <c r="L40" s="1">
+        <v>7.507943187808344E-3</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R40" s="1">
+        <v>1.1364537839676252E-4</v>
+      </c>
+      <c r="S40" s="1">
+        <v>8.5056293022214301E-5</v>
+      </c>
+      <c r="T40" s="1">
+        <v>9.4965985331142398E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+    </row>
+    <row r="42" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="I42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="Q42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1">
+        <v>22</v>
+      </c>
+      <c r="C43" s="1">
+        <v>22</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" s="1">
+        <v>22</v>
+      </c>
+      <c r="K43" s="1">
+        <v>22</v>
+      </c>
+      <c r="L43" s="1"/>
+      <c r="Q43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R43" s="1">
+        <v>22</v>
+      </c>
+      <c r="S43" s="1">
+        <v>22</v>
+      </c>
+      <c r="T43" s="1"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="1">
+        <v>200.50910980999998</v>
+      </c>
+      <c r="C44" s="1">
+        <v>208.29511796000003</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="1">
+        <v>2.3353654216268445</v>
+      </c>
+      <c r="K44" s="1">
+        <v>3.0765191699946555</v>
+      </c>
+      <c r="L44" s="1"/>
+      <c r="Q44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0.16319386387813714</v>
+      </c>
+      <c r="S44" s="1">
+        <v>0.37215031066468862</v>
+      </c>
+      <c r="T44" s="1"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="1">
+        <v>9.1140504459090899</v>
+      </c>
+      <c r="C45" s="1">
+        <v>9.4679599072727285</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="I45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.10615297371031111</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.13984178045430254</v>
+      </c>
+      <c r="L45" s="1"/>
+      <c r="Q45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R45" s="1">
+        <v>7.417902903551688E-3</v>
+      </c>
+      <c r="S45" s="1">
+        <v>1.6915923212031302E-2</v>
+      </c>
+      <c r="T45" s="1"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3.5894968998795669</v>
+      </c>
+      <c r="C46" s="1">
+        <v>6.3135782068500248</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="I46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J46" s="1">
+        <v>5.602161232331343E-3</v>
+      </c>
+      <c r="K46" s="1">
+        <v>1.0447648879663499E-2</v>
+      </c>
+      <c r="L46" s="1"/>
+      <c r="Q46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R46" s="1">
+        <v>8.0703636806039815E-5</v>
+      </c>
+      <c r="S46" s="1">
+        <v>9.3927903242805157E-4</v>
+      </c>
+      <c r="T46" s="1"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+    </row>
+    <row r="49" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T50" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U50" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="W50" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.7575483943410006</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1.7575483943410006</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.34206284066305614</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.56192572794060602</v>
+      </c>
+      <c r="G51" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J51" s="1">
+        <v>9.9878492183069767E-5</v>
+      </c>
+      <c r="K51" s="1">
+        <v>1</v>
+      </c>
+      <c r="L51" s="1">
+        <v>9.9878492183069767E-5</v>
+      </c>
+      <c r="M51" s="1">
+        <v>1.2016786412461115E-2</v>
+      </c>
+      <c r="N51" s="1">
+        <v>0.91325799880597325</v>
+      </c>
+      <c r="O51" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R51" s="1">
+        <v>8.037426272509661E-4</v>
+      </c>
+      <c r="S51" s="1">
+        <v>1</v>
+      </c>
+      <c r="T51" s="1">
+        <v>8.037426272509661E-4</v>
+      </c>
+      <c r="U51" s="1">
+        <v>1.6598709380066283</v>
+      </c>
+      <c r="V51" s="1">
+        <v>0.20502349134013664</v>
+      </c>
+      <c r="W51" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1.3777709752697831</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1.3777709752697831</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.26814866384410491</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0.60742874680731185</v>
+      </c>
+      <c r="G52" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1.2484292698173916E-2</v>
+      </c>
+      <c r="K52" s="1">
+        <v>1</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1.2484292698173916E-2</v>
+      </c>
+      <c r="M52" s="1">
+        <v>1.5020358796529132</v>
+      </c>
+      <c r="N52" s="1">
+        <v>0.22752567456955425</v>
+      </c>
+      <c r="O52" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R52" s="1">
+        <v>9.9233628758319328E-4</v>
+      </c>
+      <c r="S52" s="1">
+        <v>1</v>
+      </c>
+      <c r="T52" s="1">
+        <v>9.9233628758319328E-4</v>
+      </c>
+      <c r="U52" s="1">
+        <v>2.0493502629348699</v>
+      </c>
+      <c r="V52" s="1">
+        <v>0.16003884343386054</v>
+      </c>
+      <c r="W52" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.68357696496212839</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.68357696496212839</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.13304116074394076</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0.71722086983336153</v>
+      </c>
+      <c r="G53" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J53" s="1">
+        <v>4.4828986656532122E-3</v>
+      </c>
+      <c r="K53" s="1">
+        <v>1</v>
+      </c>
+      <c r="L53" s="1">
+        <v>4.4828986656532122E-3</v>
+      </c>
+      <c r="M53" s="1">
+        <v>0.53935571709594754</v>
+      </c>
+      <c r="N53" s="1">
+        <v>0.46698349883606294</v>
+      </c>
+      <c r="O53" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R53" s="1">
+        <v>1.2470953147781134E-3</v>
+      </c>
+      <c r="S53" s="1">
+        <v>1</v>
+      </c>
+      <c r="T53" s="1">
+        <v>1.2470953147781134E-3</v>
+      </c>
+      <c r="U53" s="1">
+        <v>2.5754727940764828</v>
+      </c>
+      <c r="V53" s="1">
+        <v>0.1163991668643751</v>
+      </c>
+      <c r="W53" s="1">
+        <v>4.0847457333016566</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="1">
+        <v>205.52345188201807</v>
+      </c>
+      <c r="C54" s="1">
+        <v>40</v>
+      </c>
+      <c r="D54" s="1">
+        <v>5.1380862970504513</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="I54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.33246323519405552</v>
+      </c>
+      <c r="K54" s="1">
+        <v>40</v>
+      </c>
+      <c r="L54" s="1">
+        <v>8.3115808798513886E-3</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="Q54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R54" s="1">
+        <v>1.9368798111886854E-2</v>
+      </c>
+      <c r="S54" s="1">
+        <v>40</v>
+      </c>
+      <c r="T54" s="1">
+        <v>4.8421995279717133E-4</v>
+      </c>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+    </row>
+    <row r="56" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="3">
+        <v>209.34234821659098</v>
+      </c>
+      <c r="C56" s="3">
+        <v>43</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="I56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0.34953030505006571</v>
+      </c>
+      <c r="K56" s="3">
+        <v>43</v>
+      </c>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="Q56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R56" s="3">
+        <v>2.2411972341499126E-2</v>
+      </c>
+      <c r="S56" s="3">
+        <v>43</v>
+      </c>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="1">
+        <v>9.1140504459090899</v>
+      </c>
+      <c r="D61" s="1">
+        <v>9.4679599072727285</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="1">
+        <v>3.5894968998795669</v>
+      </c>
+      <c r="D62" s="1">
+        <v>6.3135782068500248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" s="1">
+        <v>22</v>
+      </c>
+      <c r="D63" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0.83824832930295334</v>
+      </c>
+      <c r="D64" s="1"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="1">
+        <v>21</v>
+      </c>
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" s="1">
+        <v>-1.1973420719009309</v>
+      </c>
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0.12225728638001757</v>
+      </c>
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1.7207429028118781</v>
+      </c>
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0.24451457276003513</v>
+      </c>
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" s="3">
+        <v>2.07961384472768</v>
+      </c>
+      <c r="D71" s="3"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C76" s="1">
+        <v>9.09114452090909</v>
+      </c>
+      <c r="D76" s="1">
+        <v>9.4908658322727284</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77" s="1">
+        <v>5.0634728231494011</v>
+      </c>
+      <c r="D77" s="1">
+        <v>4.8215176445768346</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="1">
+        <v>22</v>
+      </c>
+      <c r="D78" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.75585910134643997</v>
+      </c>
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="1">
+        <v>21</v>
+      </c>
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C82" s="1">
+        <v>-1.2063099732719407</v>
+      </c>
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0.12055645715828076</v>
+      </c>
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1.7207429028118781</v>
+      </c>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0.24111291431656151</v>
+      </c>
+      <c r="D85" s="1"/>
+    </row>
+    <row r="86" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" s="3">
+        <v>2.07961384472768</v>
+      </c>
+      <c r="D86" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>